<commit_message>
reorganize input folder to fit 1 bucket and 2 buckets same type
</commit_message>
<xml_diff>
--- a/02_test4review/forReview_Burn2022Campbell.xlsx
+++ b/02_test4review/forReview_Burn2022Campbell.xlsx
@@ -34748,7 +34748,7 @@
     <row r="890">
       <c r="A890" t="inlineStr">
         <is>
-          <t>2022-06-02 00:00:00</t>
+          <t>2022-06-02 23:59:59</t>
         </is>
       </c>
       <c r="C890" t="inlineStr">
@@ -61840,7 +61840,7 @@
     <row r="1606">
       <c r="A1606" t="inlineStr">
         <is>
-          <t>2022-07-15 00:00:00</t>
+          <t>2022-07-15 23:59:59</t>
         </is>
       </c>
       <c r="C1606" t="inlineStr">
@@ -73245,7 +73245,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L80"/>
+  <dimension ref="A1:L79"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -73938,28 +73938,18 @@
     </row>
     <row r="40">
       <c r="A40" s="2">
-        <v>44714</v>
-      </c>
-      <c r="C40" t="inlineStr">
-        <is>
-          <t>Missing</t>
-        </is>
-      </c>
-      <c r="D40" t="inlineStr">
-        <is>
-          <t>Missing</t>
-        </is>
+        <v>44715</v>
       </c>
       <c r="L40">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="2">
-        <v>44715</v>
+        <v>44716</v>
       </c>
       <c r="B41">
-        <v>2.2</v>
+        <v>4</v>
       </c>
       <c r="L41">
         <v>2</v>
@@ -73967,10 +73957,10 @@
     </row>
     <row r="42">
       <c r="A42" s="2">
-        <v>44716</v>
+        <v>44717</v>
       </c>
       <c r="B42">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="L42">
         <v>2</v>
@@ -73978,10 +73968,10 @@
     </row>
     <row r="43">
       <c r="A43" s="2">
-        <v>44717</v>
+        <v>44718</v>
       </c>
       <c r="B43">
-        <v>5</v>
+        <v>1.4</v>
       </c>
       <c r="L43">
         <v>2</v>
@@ -73989,32 +73979,32 @@
     </row>
     <row r="44">
       <c r="A44" s="2">
-        <v>44718</v>
+        <v>44720</v>
       </c>
       <c r="B44">
-        <v>1.4</v>
+        <v>0.4</v>
       </c>
       <c r="L44">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="2">
-        <v>44720</v>
+        <v>44721</v>
       </c>
       <c r="B45">
-        <v>0.4</v>
+        <v>9.4</v>
       </c>
       <c r="L45">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="2">
-        <v>44721</v>
+        <v>44722</v>
       </c>
       <c r="B46">
-        <v>9.4</v>
+        <v>16</v>
       </c>
       <c r="L46">
         <v>2</v>
@@ -74022,10 +74012,10 @@
     </row>
     <row r="47">
       <c r="A47" s="2">
-        <v>44722</v>
+        <v>44723</v>
       </c>
       <c r="B47">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="L47">
         <v>2</v>
@@ -74033,10 +74023,10 @@
     </row>
     <row r="48">
       <c r="A48" s="2">
-        <v>44723</v>
+        <v>44724</v>
       </c>
       <c r="B48">
-        <v>24</v>
+        <v>15.6</v>
       </c>
       <c r="L48">
         <v>2</v>
@@ -74044,10 +74034,10 @@
     </row>
     <row r="49">
       <c r="A49" s="2">
-        <v>44724</v>
+        <v>44725</v>
       </c>
       <c r="B49">
-        <v>15.6</v>
+        <v>13.4</v>
       </c>
       <c r="L49">
         <v>2</v>
@@ -74055,10 +74045,10 @@
     </row>
     <row r="50">
       <c r="A50" s="2">
-        <v>44725</v>
+        <v>44726</v>
       </c>
       <c r="B50">
-        <v>13.4</v>
+        <v>17.2</v>
       </c>
       <c r="L50">
         <v>2</v>
@@ -74066,65 +74056,65 @@
     </row>
     <row r="51">
       <c r="A51" s="2">
-        <v>44726</v>
+        <v>44728</v>
       </c>
       <c r="B51">
-        <v>17.2</v>
+        <v>0.4</v>
       </c>
       <c r="L51">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="2">
-        <v>44728</v>
+        <v>44731</v>
       </c>
       <c r="B52">
-        <v>0.4</v>
+        <v>0.6000000000000001</v>
       </c>
       <c r="L52">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="2">
-        <v>44731</v>
+        <v>44732</v>
       </c>
       <c r="B53">
-        <v>0.6000000000000001</v>
+        <v>2</v>
       </c>
       <c r="L53">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="2">
-        <v>44732</v>
+        <v>44734</v>
       </c>
       <c r="B54">
-        <v>2</v>
+        <v>0.4</v>
       </c>
       <c r="L54">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="2">
-        <v>44734</v>
+        <v>44735</v>
       </c>
       <c r="B55">
-        <v>0.4</v>
+        <v>11</v>
       </c>
       <c r="L55">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="2">
-        <v>44735</v>
+        <v>44736</v>
       </c>
       <c r="B56">
-        <v>11</v>
+        <v>0.2</v>
       </c>
       <c r="L56">
         <v>2</v>
@@ -74132,29 +74122,39 @@
     </row>
     <row r="57">
       <c r="A57" s="2">
-        <v>44736</v>
+        <v>44740</v>
       </c>
       <c r="B57">
         <v>0.2</v>
       </c>
       <c r="L57">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="2">
-        <v>44740</v>
-      </c>
-      <c r="B58">
-        <v>0.2</v>
+        <v>44743</v>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>Missing</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>Missing</t>
+        </is>
       </c>
       <c r="L58">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="2">
-        <v>44743</v>
+        <v>44745</v>
+      </c>
+      <c r="B59">
+        <v>4.4</v>
       </c>
       <c r="C59" t="inlineStr">
         <is>
@@ -74167,15 +74167,15 @@
         </is>
       </c>
       <c r="L59">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="2">
-        <v>44745</v>
+        <v>44746</v>
       </c>
       <c r="B60">
-        <v>4.4</v>
+        <v>14.4</v>
       </c>
       <c r="C60" t="inlineStr">
         <is>
@@ -74188,15 +74188,15 @@
         </is>
       </c>
       <c r="L60">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="2">
-        <v>44746</v>
+        <v>44747</v>
       </c>
       <c r="B61">
-        <v>14.4</v>
+        <v>0.2</v>
       </c>
       <c r="C61" t="inlineStr">
         <is>
@@ -74214,10 +74214,10 @@
     </row>
     <row r="62">
       <c r="A62" s="2">
-        <v>44747</v>
+        <v>44748</v>
       </c>
       <c r="B62">
-        <v>0.2</v>
+        <v>0.4</v>
       </c>
       <c r="C62" t="inlineStr">
         <is>
@@ -74235,10 +74235,10 @@
     </row>
     <row r="63">
       <c r="A63" s="2">
-        <v>44748</v>
+        <v>44749</v>
       </c>
       <c r="B63">
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="C63" t="inlineStr">
         <is>
@@ -74256,10 +74256,7 @@
     </row>
     <row r="64">
       <c r="A64" s="2">
-        <v>44749</v>
-      </c>
-      <c r="B64">
-        <v>0.2</v>
+        <v>44758</v>
       </c>
       <c r="C64" t="inlineStr">
         <is>
@@ -74272,110 +74269,103 @@
         </is>
       </c>
       <c r="L64">
-        <v>2</v>
+        <v>10</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="2">
-        <v>44757</v>
-      </c>
-      <c r="C65" t="inlineStr">
-        <is>
-          <t>Missing</t>
-        </is>
-      </c>
-      <c r="D65" t="inlineStr">
-        <is>
-          <t>Missing</t>
-        </is>
+        <v>44760</v>
+      </c>
+      <c r="B65">
+        <v>4.4</v>
       </c>
       <c r="L65">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="2">
-        <v>44760</v>
+        <v>44777</v>
       </c>
       <c r="B66">
-        <v>4.4</v>
+        <v>3.2</v>
       </c>
       <c r="L66">
-        <v>4</v>
+        <v>18</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="2">
-        <v>44777</v>
+        <v>44778</v>
       </c>
       <c r="B67">
-        <v>3.2</v>
+        <v>2.6</v>
       </c>
       <c r="L67">
-        <v>18</v>
+        <v>2</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="2">
-        <v>44778</v>
+        <v>44781</v>
       </c>
       <c r="B68">
-        <v>2.6</v>
+        <v>0.2</v>
       </c>
       <c r="L68">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="2">
-        <v>44781</v>
+        <v>44785</v>
       </c>
       <c r="B69">
-        <v>0.2</v>
+        <v>1.6</v>
       </c>
       <c r="L69">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="2">
-        <v>44785</v>
+        <v>44786</v>
       </c>
       <c r="B70">
-        <v>1.6</v>
+        <v>1</v>
       </c>
       <c r="L70">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="2">
-        <v>44786</v>
+        <v>44798</v>
       </c>
       <c r="B71">
-        <v>1</v>
+        <v>3.8</v>
       </c>
       <c r="L71">
-        <v>2</v>
+        <v>13</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="2">
-        <v>44798</v>
+        <v>44799</v>
       </c>
       <c r="B72">
-        <v>3.8</v>
+        <v>0.6000000000000001</v>
       </c>
       <c r="L72">
-        <v>13</v>
+        <v>2</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="2">
-        <v>44799</v>
+        <v>44800</v>
       </c>
       <c r="B73">
-        <v>0.6000000000000001</v>
+        <v>5.4</v>
       </c>
       <c r="L73">
         <v>2</v>
@@ -74383,32 +74373,32 @@
     </row>
     <row r="74">
       <c r="A74" s="2">
-        <v>44800</v>
+        <v>44818</v>
       </c>
       <c r="B74">
-        <v>5.4</v>
+        <v>10.4</v>
       </c>
       <c r="L74">
-        <v>2</v>
+        <v>19</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="2">
-        <v>44818</v>
+        <v>44819</v>
       </c>
       <c r="B75">
-        <v>10.4</v>
+        <v>5.800000000000001</v>
       </c>
       <c r="L75">
-        <v>19</v>
+        <v>2</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="2">
-        <v>44819</v>
+        <v>44820</v>
       </c>
       <c r="B76">
-        <v>5.800000000000001</v>
+        <v>9.4</v>
       </c>
       <c r="L76">
         <v>2</v>
@@ -74416,10 +74406,10 @@
     </row>
     <row r="77">
       <c r="A77" s="2">
-        <v>44820</v>
+        <v>44821</v>
       </c>
       <c r="B77">
-        <v>9.4</v>
+        <v>9</v>
       </c>
       <c r="L77">
         <v>2</v>
@@ -74427,34 +74417,23 @@
     </row>
     <row r="78">
       <c r="A78" s="2">
-        <v>44821</v>
+        <v>44833</v>
       </c>
       <c r="B78">
-        <v>9</v>
+        <v>2.8</v>
       </c>
       <c r="L78">
-        <v>2</v>
+        <v>13</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="2">
-        <v>44833</v>
+        <v>44845</v>
       </c>
       <c r="B79">
-        <v>2.8</v>
+        <v>4</v>
       </c>
       <c r="L79">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="80">
-      <c r="A80" s="2">
-        <v>44845</v>
-      </c>
-      <c r="B80">
-        <v>4</v>
-      </c>
-      <c r="L80">
         <v>13</v>
       </c>
     </row>

</xml_diff>